<commit_message>
annotation update, finalList incomplete
</commit_message>
<xml_diff>
--- a/Datasets/Annotated/Annotated_Amazon_Reviews.xlsx
+++ b/Datasets/Annotated/Annotated_Amazon_Reviews.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuangDaoVuNgoc\github\bachelorthesis\Datasets\Annotated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8FFC0B-3FF2-4087-97BE-A4D42AFC1908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0AA11B2-A002-40D7-9915-AE59255F03A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$1001</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -6778,8 +6781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A241" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A174" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B224" sqref="B224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6817,29 +6820,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2101</v>
-      </c>
-      <c r="E2">
-        <f>COUNTIF(C2:C1001,1)</f>
-        <v>151</v>
-      </c>
-      <c r="F2">
-        <f>COUNTIF(C2:C1001,2)</f>
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <f>COUNTIF(C2:C1001,3)</f>
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <f>COUNTIF(C2:C1001,0)</f>
-        <v>71</v>
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6847,18 +6834,18 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>1.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -6866,10 +6853,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -6880,21 +6867,21 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -6902,10 +6889,10 @@
         <v>-1</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -6913,10 +6900,10 @@
         <v>-1</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -6924,21 +6911,21 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>2104</v>
+        <v>28</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -6946,7 +6933,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -6954,24 +6941,24 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>2105</v>
+        <v>34</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -6979,18 +6966,18 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -6998,13 +6985,13 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -7012,10 +6999,10 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -7023,7 +7010,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -7034,7 +7021,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -7045,7 +7032,7 @@
         <v>-1</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -7053,24 +7040,24 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -7078,21 +7065,21 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -7100,7 +7087,7 @@
         <v>-1</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>102</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -7111,29 +7098,29 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>111</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>116</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>117</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -7141,13 +7128,13 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -7155,7 +7142,7 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -7166,10 +7153,10 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -7177,10 +7164,10 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -7188,7 +7175,7 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -7196,10 +7183,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>129</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -7210,10 +7197,10 @@
         <v>-1</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>130</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -7221,7 +7208,7 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>139</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -7229,24 +7216,24 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>150</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -7254,21 +7241,21 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>153</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>160</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -7276,7 +7263,7 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>161</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -7287,10 +7274,10 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>165</v>
       </c>
       <c r="C43">
-        <v>1.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -7298,10 +7285,10 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>166</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -7309,43 +7296,43 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>167</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>169</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>46</v>
+        <v>170</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
+        <v>171</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -7353,10 +7340,10 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>48</v>
+        <v>173</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -7364,10 +7351,10 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>177</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -7375,32 +7362,32 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>50</v>
+        <v>185</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>51</v>
+        <v>186</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="C53">
-        <v>1.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -7408,18 +7395,18 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>53</v>
+        <v>190</v>
       </c>
       <c r="C54">
-        <v>1.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B55" t="s">
-        <v>54</v>
+        <v>196</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -7430,10 +7417,10 @@
         <v>-1</v>
       </c>
       <c r="B56" t="s">
-        <v>55</v>
+        <v>202</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -7441,7 +7428,7 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>56</v>
+        <v>205</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -7452,10 +7439,10 @@
         <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>57</v>
+        <v>212</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -7463,7 +7450,7 @@
         <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>58</v>
+        <v>216</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -7471,13 +7458,13 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B60" t="s">
-        <v>59</v>
+        <v>217</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -7485,10 +7472,10 @@
         <v>-1</v>
       </c>
       <c r="B61" t="s">
-        <v>60</v>
+        <v>218</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -7496,21 +7483,21 @@
         <v>1</v>
       </c>
       <c r="B62" t="s">
-        <v>61</v>
+        <v>223</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B63" t="s">
-        <v>62</v>
+        <v>224</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -7518,21 +7505,21 @@
         <v>-1</v>
       </c>
       <c r="B64" t="s">
-        <v>63</v>
+        <v>225</v>
       </c>
       <c r="C64">
-        <v>1.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B65" t="s">
-        <v>64</v>
+        <v>226</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -7540,21 +7527,21 @@
         <v>1</v>
       </c>
       <c r="B66" t="s">
-        <v>65</v>
+        <v>228</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B67" t="s">
-        <v>66</v>
+        <v>234</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -7562,10 +7549,10 @@
         <v>-1</v>
       </c>
       <c r="B68" t="s">
-        <v>67</v>
+        <v>235</v>
       </c>
       <c r="C68">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -7573,10 +7560,10 @@
         <v>1</v>
       </c>
       <c r="B69" t="s">
-        <v>68</v>
+        <v>237</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -7584,7 +7571,7 @@
         <v>1</v>
       </c>
       <c r="B70" t="s">
-        <v>69</v>
+        <v>240</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -7595,7 +7582,7 @@
         <v>1</v>
       </c>
       <c r="B71" t="s">
-        <v>70</v>
+        <v>241</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -7603,21 +7590,21 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B72" t="s">
-        <v>71</v>
+        <v>248</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B73" t="s">
-        <v>72</v>
+        <v>6</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -7628,7 +7615,7 @@
         <v>-1</v>
       </c>
       <c r="B74" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -7639,7 +7626,7 @@
         <v>-1</v>
       </c>
       <c r="B75" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -7647,10 +7634,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B76" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -7661,10 +7648,10 @@
         <v>-1</v>
       </c>
       <c r="B77" t="s">
-        <v>76</v>
+        <v>11</v>
       </c>
       <c r="C77">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -7672,7 +7659,7 @@
         <v>-1</v>
       </c>
       <c r="B78" t="s">
-        <v>77</v>
+        <v>2105</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -7683,10 +7670,10 @@
         <v>-1</v>
       </c>
       <c r="B79" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -7694,7 +7681,7 @@
         <v>1</v>
       </c>
       <c r="B80" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -7702,13 +7689,13 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B81" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -7716,7 +7703,7 @@
         <v>1</v>
       </c>
       <c r="B82" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -7727,10 +7714,10 @@
         <v>-1</v>
       </c>
       <c r="B83" t="s">
-        <v>82</v>
+        <v>21</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -7738,7 +7725,7 @@
         <v>-1</v>
       </c>
       <c r="B84" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -7746,10 +7733,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B85" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="C85">
         <v>1</v>
@@ -7757,10 +7744,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B86" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -7771,7 +7758,7 @@
         <v>-1</v>
       </c>
       <c r="B87" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="C87">
         <v>1</v>
@@ -7782,18 +7769,18 @@
         <v>1</v>
       </c>
       <c r="B88" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
       <c r="C88">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B89" t="s">
-        <v>88</v>
+        <v>32</v>
       </c>
       <c r="C89">
         <v>1</v>
@@ -7804,7 +7791,7 @@
         <v>-1</v>
       </c>
       <c r="B90" t="s">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="C90">
         <v>1</v>
@@ -7812,10 +7799,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B91" t="s">
-        <v>90</v>
+        <v>37</v>
       </c>
       <c r="C91">
         <v>1</v>
@@ -7823,10 +7810,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B92" t="s">
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="C92">
         <v>1</v>
@@ -7834,10 +7821,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B93" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="C93">
         <v>1</v>
@@ -7845,10 +7832,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B94" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="C94">
         <v>1</v>
@@ -7859,7 +7846,7 @@
         <v>1</v>
       </c>
       <c r="B95" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="C95">
         <v>1</v>
@@ -7867,10 +7854,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B96" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="C96">
         <v>1</v>
@@ -7878,10 +7865,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B97" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="C97">
         <v>1</v>
@@ -7892,7 +7879,7 @@
         <v>-1</v>
       </c>
       <c r="B98" t="s">
-        <v>97</v>
+        <v>46</v>
       </c>
       <c r="C98">
         <v>1</v>
@@ -7900,21 +7887,21 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B99" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B100" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="C100">
         <v>1</v>
@@ -7925,18 +7912,18 @@
         <v>1</v>
       </c>
       <c r="B101" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B102" t="s">
-        <v>101</v>
+        <v>50</v>
       </c>
       <c r="C102">
         <v>1</v>
@@ -7947,10 +7934,10 @@
         <v>-1</v>
       </c>
       <c r="B103" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="C103">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -7958,21 +7945,21 @@
         <v>-1</v>
       </c>
       <c r="B104" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
       <c r="C104">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B105" t="s">
-        <v>104</v>
+        <v>57</v>
       </c>
       <c r="C105">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -7980,10 +7967,10 @@
         <v>1</v>
       </c>
       <c r="B106" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="C106">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -7991,18 +7978,18 @@
         <v>-1</v>
       </c>
       <c r="B107" t="s">
-        <v>106</v>
+        <v>60</v>
       </c>
       <c r="C107">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B108" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="C108">
         <v>1</v>
@@ -8013,7 +8000,7 @@
         <v>-1</v>
       </c>
       <c r="B109" t="s">
-        <v>108</v>
+        <v>62</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -8021,13 +8008,13 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B110" t="s">
-        <v>109</v>
+        <v>64</v>
       </c>
       <c r="C110">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -8035,7 +8022,7 @@
         <v>1</v>
       </c>
       <c r="B111" t="s">
-        <v>110</v>
+        <v>65</v>
       </c>
       <c r="C111">
         <v>1</v>
@@ -8043,21 +8030,21 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B112" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
       <c r="C112">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B113" t="s">
-        <v>112</v>
+        <v>67</v>
       </c>
       <c r="C113">
         <v>1</v>
@@ -8068,7 +8055,7 @@
         <v>1</v>
       </c>
       <c r="B114" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
       <c r="C114">
         <v>1</v>
@@ -8076,10 +8063,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B115" t="s">
-        <v>114</v>
+        <v>71</v>
       </c>
       <c r="C115">
         <v>1</v>
@@ -8090,7 +8077,7 @@
         <v>-1</v>
       </c>
       <c r="B116" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="C116">
         <v>1</v>
@@ -8098,13 +8085,13 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B117" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -8112,10 +8099,10 @@
         <v>-1</v>
       </c>
       <c r="B118" t="s">
-        <v>117</v>
+        <v>74</v>
       </c>
       <c r="C118">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -8123,7 +8110,7 @@
         <v>1</v>
       </c>
       <c r="B119" t="s">
-        <v>118</v>
+        <v>75</v>
       </c>
       <c r="C119">
         <v>1</v>
@@ -8131,13 +8118,13 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B120" t="s">
-        <v>119</v>
+        <v>77</v>
       </c>
       <c r="C120">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -8145,10 +8132,10 @@
         <v>1</v>
       </c>
       <c r="B121" t="s">
-        <v>120</v>
+        <v>79</v>
       </c>
       <c r="C121">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -8156,7 +8143,7 @@
         <v>1</v>
       </c>
       <c r="B122" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="C122">
         <v>1</v>
@@ -8164,10 +8151,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B123" t="s">
-        <v>122</v>
+        <v>83</v>
       </c>
       <c r="C123">
         <v>1</v>
@@ -8175,13 +8162,13 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B124" t="s">
-        <v>123</v>
+        <v>84</v>
       </c>
       <c r="C124">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -8189,7 +8176,7 @@
         <v>1</v>
       </c>
       <c r="B125" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="C125">
         <v>1</v>
@@ -8197,21 +8184,21 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B126" t="s">
-        <v>125</v>
+        <v>86</v>
       </c>
       <c r="C126">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B127" t="s">
-        <v>126</v>
+        <v>88</v>
       </c>
       <c r="C127">
         <v>1</v>
@@ -8219,10 +8206,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B128" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="C128">
         <v>1</v>
@@ -8233,10 +8220,10 @@
         <v>1</v>
       </c>
       <c r="B129" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -8244,10 +8231,10 @@
         <v>-1</v>
       </c>
       <c r="B130" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="C130">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -8255,10 +8242,10 @@
         <v>-1</v>
       </c>
       <c r="B131" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -8266,7 +8253,7 @@
         <v>1</v>
       </c>
       <c r="B132" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="C132">
         <v>1</v>
@@ -8277,18 +8264,18 @@
         <v>1</v>
       </c>
       <c r="B133" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="C133">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B134" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="C134">
         <v>1</v>
@@ -8299,21 +8286,21 @@
         <v>1</v>
       </c>
       <c r="B135" t="s">
-        <v>134</v>
+        <v>96</v>
       </c>
       <c r="C135">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B136" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="C136">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -8321,10 +8308,10 @@
         <v>-1</v>
       </c>
       <c r="B137" t="s">
-        <v>136</v>
+        <v>99</v>
       </c>
       <c r="C137">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -8332,7 +8319,7 @@
         <v>-1</v>
       </c>
       <c r="B138" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
       <c r="C138">
         <v>1</v>
@@ -8340,10 +8327,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B139" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
       <c r="C139">
         <v>1</v>
@@ -8351,21 +8338,21 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B140" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B141" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="C141">
         <v>1</v>
@@ -8373,10 +8360,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B142" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="C142">
         <v>1</v>
@@ -8384,13 +8371,13 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B143" t="s">
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="C143">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -8398,21 +8385,21 @@
         <v>1</v>
       </c>
       <c r="B144" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="C144">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B145" t="s">
-        <v>144</v>
-      </c>
-      <c r="C145" t="s">
-        <v>2106</v>
+        <v>115</v>
+      </c>
+      <c r="C145">
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -8420,7 +8407,7 @@
         <v>1</v>
       </c>
       <c r="B146" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="C146">
         <v>1</v>
@@ -8428,10 +8415,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B147" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="C147">
         <v>1</v>
@@ -8442,7 +8429,7 @@
         <v>1</v>
       </c>
       <c r="B148" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="C148">
         <v>1</v>
@@ -8450,43 +8437,43 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B149" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="C149">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B150" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="C150">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B151" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="C151">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B152" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="C152">
         <v>1</v>
@@ -8497,7 +8484,7 @@
         <v>1</v>
       </c>
       <c r="B153" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="C153">
         <v>1</v>
@@ -8505,13 +8492,13 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B154" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="C154">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -8519,7 +8506,7 @@
         <v>1</v>
       </c>
       <c r="B155" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="C155">
         <v>1</v>
@@ -8530,7 +8517,7 @@
         <v>-1</v>
       </c>
       <c r="B156" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="C156">
         <v>1</v>
@@ -8538,10 +8525,10 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B157" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="C157">
         <v>1</v>
@@ -8552,7 +8539,7 @@
         <v>1</v>
       </c>
       <c r="B158" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C158">
         <v>1</v>
@@ -8560,13 +8547,13 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B159" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C159">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -8574,21 +8561,21 @@
         <v>1</v>
       </c>
       <c r="B160" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C160">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B161" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C161">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -8596,10 +8583,10 @@
         <v>1</v>
       </c>
       <c r="B162" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C162">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -8607,7 +8594,7 @@
         <v>1</v>
       </c>
       <c r="B163" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C163">
         <v>1</v>
@@ -8615,10 +8602,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B164" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C164">
         <v>1</v>
@@ -8626,10 +8613,10 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B165" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C165">
         <v>1</v>
@@ -8640,10 +8627,10 @@
         <v>1</v>
       </c>
       <c r="B166" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C166">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -8651,10 +8638,10 @@
         <v>1</v>
       </c>
       <c r="B167" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C167">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -8662,10 +8649,10 @@
         <v>1</v>
       </c>
       <c r="B168" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C168">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -8673,7 +8660,7 @@
         <v>-1</v>
       </c>
       <c r="B169" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C169">
         <v>1</v>
@@ -8681,35 +8668,35 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B170" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C170">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B171" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C171">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B172" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C172">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -8717,7 +8704,7 @@
         <v>-1</v>
       </c>
       <c r="B173" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C173">
         <v>1</v>
@@ -8725,13 +8712,13 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B174" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C174">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -8739,7 +8726,7 @@
         <v>-1</v>
       </c>
       <c r="B175" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="C175">
         <v>1</v>
@@ -8750,7 +8737,7 @@
         <v>-1</v>
       </c>
       <c r="B176" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C176">
         <v>1</v>
@@ -8761,7 +8748,7 @@
         <v>-1</v>
       </c>
       <c r="B177" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C177">
         <v>1</v>
@@ -8769,13 +8756,13 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B178" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C178">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -8783,10 +8770,10 @@
         <v>-1</v>
       </c>
       <c r="B179" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C179">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -8794,7 +8781,7 @@
         <v>-1</v>
       </c>
       <c r="B180" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C180">
         <v>1</v>
@@ -8805,7 +8792,7 @@
         <v>-1</v>
       </c>
       <c r="B181" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="C181">
         <v>1</v>
@@ -8816,7 +8803,7 @@
         <v>-1</v>
       </c>
       <c r="B182" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="C182">
         <v>1</v>
@@ -8827,7 +8814,7 @@
         <v>-1</v>
       </c>
       <c r="B183" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="C183">
         <v>1</v>
@@ -8835,10 +8822,10 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B184" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="C184">
         <v>1</v>
@@ -8849,7 +8836,7 @@
         <v>-1</v>
       </c>
       <c r="B185" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="C185">
         <v>1</v>
@@ -8860,21 +8847,21 @@
         <v>1</v>
       </c>
       <c r="B186" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="C186">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B187" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="C187">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -8882,7 +8869,7 @@
         <v>-1</v>
       </c>
       <c r="B188" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="C188">
         <v>1</v>
@@ -8893,10 +8880,10 @@
         <v>1</v>
       </c>
       <c r="B189" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="C189">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -8904,7 +8891,7 @@
         <v>-1</v>
       </c>
       <c r="B190" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C190">
         <v>1</v>
@@ -8915,10 +8902,10 @@
         <v>1</v>
       </c>
       <c r="B191" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="C191">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -8926,7 +8913,7 @@
         <v>-1</v>
       </c>
       <c r="B192" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="C192">
         <v>1</v>
@@ -8934,10 +8921,10 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B193" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="C193">
         <v>1</v>
@@ -8945,10 +8932,10 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B194" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="C194">
         <v>1</v>
@@ -8959,7 +8946,7 @@
         <v>1</v>
       </c>
       <c r="B195" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C195">
         <v>1</v>
@@ -8970,7 +8957,7 @@
         <v>-1</v>
       </c>
       <c r="B196" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="C196">
         <v>1</v>
@@ -8981,10 +8968,10 @@
         <v>-1</v>
       </c>
       <c r="B197" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="C197">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -8992,7 +8979,7 @@
         <v>-1</v>
       </c>
       <c r="B198" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="C198">
         <v>1</v>
@@ -9000,10 +8987,10 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B199" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="C199">
         <v>1</v>
@@ -9014,7 +9001,7 @@
         <v>-1</v>
       </c>
       <c r="B200" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
       <c r="C200">
         <v>1</v>
@@ -9025,7 +9012,7 @@
         <v>1</v>
       </c>
       <c r="B201" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="C201">
         <v>1</v>
@@ -9033,10 +9020,10 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B202" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="C202">
         <v>1</v>
@@ -9047,18 +9034,18 @@
         <v>-1</v>
       </c>
       <c r="B203" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="C203">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B204" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="C204">
         <v>1</v>
@@ -9069,7 +9056,7 @@
         <v>1</v>
       </c>
       <c r="B205" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
       <c r="C205">
         <v>1</v>
@@ -9077,13 +9064,13 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B206" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
       <c r="C206">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -9091,7 +9078,7 @@
         <v>1</v>
       </c>
       <c r="B207" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="C207">
         <v>1</v>
@@ -9099,10 +9086,10 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B208" t="s">
-        <v>207</v>
+        <v>229</v>
       </c>
       <c r="C208">
         <v>1</v>
@@ -9113,7 +9100,7 @@
         <v>-1</v>
       </c>
       <c r="B209" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="C209">
         <v>1</v>
@@ -9124,10 +9111,10 @@
         <v>1</v>
       </c>
       <c r="B210" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="C210">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -9135,7 +9122,7 @@
         <v>-1</v>
       </c>
       <c r="B211" t="s">
-        <v>210</v>
+        <v>232</v>
       </c>
       <c r="C211">
         <v>1</v>
@@ -9146,7 +9133,7 @@
         <v>-1</v>
       </c>
       <c r="B212" t="s">
-        <v>211</v>
+        <v>233</v>
       </c>
       <c r="C212">
         <v>1</v>
@@ -9157,10 +9144,10 @@
         <v>1</v>
       </c>
       <c r="B213" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="C213">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -9168,7 +9155,7 @@
         <v>-1</v>
       </c>
       <c r="B214" t="s">
-        <v>213</v>
+        <v>239</v>
       </c>
       <c r="C214">
         <v>1</v>
@@ -9179,7 +9166,7 @@
         <v>1</v>
       </c>
       <c r="B215" t="s">
-        <v>214</v>
+        <v>242</v>
       </c>
       <c r="C215">
         <v>1</v>
@@ -9190,7 +9177,7 @@
         <v>1</v>
       </c>
       <c r="B216" t="s">
-        <v>215</v>
+        <v>243</v>
       </c>
       <c r="C216">
         <v>1</v>
@@ -9201,40 +9188,40 @@
         <v>1</v>
       </c>
       <c r="B217" t="s">
-        <v>216</v>
+        <v>244</v>
       </c>
       <c r="C217">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B218" t="s">
-        <v>217</v>
+        <v>245</v>
       </c>
       <c r="C218">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B219" t="s">
-        <v>218</v>
+        <v>246</v>
       </c>
       <c r="C219">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B220" t="s">
-        <v>219</v>
+        <v>247</v>
       </c>
       <c r="C220">
         <v>1</v>
@@ -9242,10 +9229,10 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B221" t="s">
-        <v>220</v>
+        <v>249</v>
       </c>
       <c r="C221">
         <v>1</v>
@@ -9256,7 +9243,7 @@
         <v>1</v>
       </c>
       <c r="B222" t="s">
-        <v>221</v>
+        <v>250</v>
       </c>
       <c r="C222">
         <v>1</v>
@@ -9267,7 +9254,7 @@
         <v>-1</v>
       </c>
       <c r="B223" t="s">
-        <v>222</v>
+        <v>251</v>
       </c>
       <c r="C223">
         <v>1</v>
@@ -9278,10 +9265,10 @@
         <v>1</v>
       </c>
       <c r="B224" t="s">
-        <v>223</v>
+        <v>42</v>
       </c>
       <c r="C224">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -9289,10 +9276,10 @@
         <v>1</v>
       </c>
       <c r="B225" t="s">
-        <v>224</v>
+        <v>53</v>
       </c>
       <c r="C225">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -9300,10 +9287,10 @@
         <v>-1</v>
       </c>
       <c r="B226" t="s">
-        <v>225</v>
+        <v>63</v>
       </c>
       <c r="C226">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
@@ -9311,32 +9298,32 @@
         <v>-1</v>
       </c>
       <c r="B227" t="s">
-        <v>226</v>
+        <v>76</v>
       </c>
       <c r="C227">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B228" t="s">
-        <v>227</v>
+        <v>103</v>
       </c>
       <c r="C228">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B229" t="s">
-        <v>228</v>
+        <v>104</v>
       </c>
       <c r="C229">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
@@ -9344,10 +9331,10 @@
         <v>1</v>
       </c>
       <c r="B230" t="s">
-        <v>229</v>
+        <v>105</v>
       </c>
       <c r="C230">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -9355,43 +9342,43 @@
         <v>-1</v>
       </c>
       <c r="B231" t="s">
-        <v>230</v>
+        <v>106</v>
       </c>
       <c r="C231">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B232" t="s">
-        <v>231</v>
+        <v>109</v>
       </c>
       <c r="C232">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B233" t="s">
-        <v>232</v>
+        <v>132</v>
       </c>
       <c r="C233">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B234" t="s">
-        <v>233</v>
+        <v>134</v>
       </c>
       <c r="C234">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -9399,10 +9386,10 @@
         <v>1</v>
       </c>
       <c r="B235" t="s">
-        <v>234</v>
+        <v>135</v>
       </c>
       <c r="C235">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -9410,21 +9397,21 @@
         <v>-1</v>
       </c>
       <c r="B236" t="s">
-        <v>235</v>
+        <v>136</v>
       </c>
       <c r="C236">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B237" t="s">
-        <v>236</v>
+        <v>148</v>
       </c>
       <c r="C237">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -9432,10 +9419,10 @@
         <v>1</v>
       </c>
       <c r="B238" t="s">
-        <v>237</v>
+        <v>158</v>
       </c>
       <c r="C238">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -9443,156 +9430,172 @@
         <v>1</v>
       </c>
       <c r="B239" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
       <c r="C239">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B240" t="s">
-        <v>239</v>
+        <v>3</v>
       </c>
       <c r="C240">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B241" t="s">
-        <v>240</v>
+        <v>52</v>
       </c>
       <c r="C241">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>-1</v>
+      </c>
+      <c r="B242" t="s">
+        <v>142</v>
+      </c>
+      <c r="C242">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>-1</v>
+      </c>
+      <c r="B243" t="s">
+        <v>149</v>
+      </c>
+      <c r="C243">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>1</v>
+      </c>
+      <c r="B244" t="s">
+        <v>159</v>
+      </c>
+      <c r="C244">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>-1</v>
+      </c>
+      <c r="B245" t="s">
+        <v>178</v>
+      </c>
+      <c r="C245">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>1</v>
+      </c>
+      <c r="B246" t="s">
+        <v>238</v>
+      </c>
+      <c r="C246">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>1</v>
+      </c>
+      <c r="B247" t="s">
+        <v>22</v>
+      </c>
+      <c r="C247">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>1</v>
+      </c>
+      <c r="B248" t="s">
+        <v>23</v>
+      </c>
+      <c r="C248">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>1</v>
+      </c>
+      <c r="B249" t="s">
+        <v>87</v>
+      </c>
+      <c r="C249">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>1</v>
+      </c>
+      <c r="B250" t="s">
+        <v>2</v>
+      </c>
+      <c r="C250" t="s">
+        <v>2101</v>
+      </c>
+      <c r="E250">
+        <f>COUNTIF(C250:C1249,1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A242">
-        <v>1</v>
-      </c>
-      <c r="B242" t="s">
-        <v>241</v>
-      </c>
-      <c r="C242">
+      <c r="F250">
+        <f>COUNTIF(C250:C1249,2)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A243">
-        <v>1</v>
-      </c>
-      <c r="B243" t="s">
-        <v>242</v>
-      </c>
-      <c r="C243">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A244">
-        <v>1</v>
-      </c>
-      <c r="B244" t="s">
-        <v>243</v>
-      </c>
-      <c r="C244">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A245">
-        <v>1</v>
-      </c>
-      <c r="B245" t="s">
-        <v>244</v>
-      </c>
-      <c r="C245">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A246">
-        <v>1</v>
-      </c>
-      <c r="B246" t="s">
-        <v>245</v>
-      </c>
-      <c r="C246">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A247">
-        <v>1</v>
-      </c>
-      <c r="B247" t="s">
-        <v>246</v>
-      </c>
-      <c r="C247">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A248">
-        <v>1</v>
-      </c>
-      <c r="B248" t="s">
-        <v>247</v>
-      </c>
-      <c r="C248">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A249">
-        <v>1</v>
-      </c>
-      <c r="B249" t="s">
-        <v>248</v>
-      </c>
-      <c r="C249">
+      <c r="G250">
+        <f>COUNTIF(C250:C1249,3)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A250">
-        <v>-1</v>
-      </c>
-      <c r="B250" t="s">
-        <v>249</v>
-      </c>
-      <c r="C250">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H250">
+        <f>COUNTIF(C250:C1249,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>1</v>
       </c>
       <c r="B251" t="s">
-        <v>250</v>
-      </c>
-      <c r="C251">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C251" t="s">
+        <v>2104</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B252" t="s">
-        <v>251</v>
-      </c>
-      <c r="C252">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="C252" t="s">
+        <v>2106</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>1</v>
       </c>
@@ -9600,7 +9603,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>1</v>
       </c>
@@ -9608,7 +9611,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>-1</v>
       </c>
@@ -9616,7 +9619,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>-1</v>
       </c>
@@ -15585,6 +15588,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H1001">
+    <sortCondition ref="C2:C1001"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
results of annotation check (w/o calc as of now)
</commit_message>
<xml_diff>
--- a/Datasets/Annotated/Annotated_Amazon_Reviews.xlsx
+++ b/Datasets/Annotated/Annotated_Amazon_Reviews.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuangDaoVuNgoc\github\bachelorthesis\Datasets\Annotated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0AA11B2-A002-40D7-9915-AE59255F03A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA73393-23FB-46A5-B503-CC04F8545B2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6781,8 +6781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B224" sqref="B224"/>
+    <sheetView tabSelected="1" topLeftCell="A265" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B282" sqref="B282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6828,6 +6828,22 @@
       <c r="C2">
         <v>0</v>
       </c>
+      <c r="E2">
+        <f>COUNTIF(C2:C1001,1)</f>
+        <v>152</v>
+      </c>
+      <c r="F2">
+        <f>COUNTIF(C2:C1001,2)</f>
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <f>COUNTIF(C2:C1001,3)</f>
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <f>COUNTIF(C2:C1001,0)</f>
+        <v>71</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -9447,7 +9463,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>-1</v>
       </c>
@@ -9458,7 +9474,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>-1</v>
       </c>
@@ -9469,7 +9485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>-1</v>
       </c>
@@ -9480,7 +9496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>1</v>
       </c>
@@ -9491,7 +9507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>-1</v>
       </c>
@@ -9502,7 +9518,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>1</v>
       </c>
@@ -9513,7 +9529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>1</v>
       </c>
@@ -9524,7 +9540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>1</v>
       </c>
@@ -9535,7 +9551,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>1</v>
       </c>
@@ -9546,7 +9562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>1</v>
       </c>
@@ -9556,24 +9572,8 @@
       <c r="C250" t="s">
         <v>2101</v>
       </c>
-      <c r="E250">
-        <f>COUNTIF(C250:C1249,1)</f>
-        <v>0</v>
-      </c>
-      <c r="F250">
-        <f>COUNTIF(C250:C1249,2)</f>
-        <v>0</v>
-      </c>
-      <c r="G250">
-        <f>COUNTIF(C250:C1249,3)</f>
-        <v>0</v>
-      </c>
-      <c r="H250">
-        <f>COUNTIF(C250:C1249,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>1</v>
       </c>
@@ -9584,7 +9584,7 @@
         <v>2104</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>1</v>
       </c>
@@ -9595,7 +9595,7 @@
         <v>2106</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>1</v>
       </c>
@@ -9603,7 +9603,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>1</v>
       </c>
@@ -9611,7 +9611,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>-1</v>
       </c>
@@ -9619,7 +9619,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>-1</v>
       </c>

</xml_diff>